<commit_message>
problème de lois reglé!
</commit_message>
<xml_diff>
--- a/data/lois_duree.xlsx
+++ b/data/lois_duree.xlsx
@@ -436,27 +436,27 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Rue</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Entreprise</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Sans</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Domicile</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Parking</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Domicile</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Sans</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Rue</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Entreprise</t>
         </is>
       </c>
     </row>
@@ -468,27 +468,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['invgamma', (1.390737571634801, -9.772127964194171e-31, 1.7259786363251786)]</t>
+          <t>['invgauss', (4.036204719120207, -0.16161763541930152, 0.9612597581681632)]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['beta', (2.1872413962120696, -0.005988001327689882, 3.6925482232686946)]</t>
+          <t>['beta', (52.595462995358545, 27.703319219454222, -35.25571817939934, 64.73662886568977)]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['beta', (1.218287798623423, -5.139663880520553e-31, 2.818723489330444)]</t>
+          <t>['beta', (0.5117940197816365, 19.2230902247954, -5.458435128107077e-24, 16.73836142353016)]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['invgauss', (1.3395802550303704, -1.7904907549755111e-28, 1.853609719131836)]</t>
+          <t>['beta', (0.5474258078179828, 0.9000121427405545, -3.7860672030373568e-28, 21.599798314360253)]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['loggamma', (200.9195815067319, -27.948438121633316, 0.17453264527549273)]</t>
+          <t>['invgamma', (1.2485500680449202, -0.23360330017153055, 1.298576682245404)]</t>
         </is>
       </c>
     </row>
@@ -500,27 +500,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['pareto', (1.4013317752688952, -1.0965230799343156e-28, 1.6534975834359054)]</t>
+          <t>['chi2', (1.3400808769713695, -5.127648667537803e-29, 1.8549957545294835)]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['beta', (1.450000395484929, -2.2827792178756118e-28, 1.7333331911256646)]</t>
+          <t>['invgamma', (54.707261432752674, -13.673652829752161, 977.6742062851458)]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['beta', (1.2651197309118647, -1.9934723799161143e-29, 3.255682061478039)]</t>
+          <t>['beta', (0.30450496225678947, 88.52544141212059, -3.1546313693862455e-28, 176.8979751292736)]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['chi2', (1.3400808769713695, -5.127648667537803e-29, 1.8549957545294835)]</t>
+          <t>['beta', (0.547862902931137, 0.6163748511340661, -4.316342930087755e-25, 12.900063624422803)]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['invgamma', (23.59867259214333, -4.10339870239223, 0.36582546125820503)]</t>
+          <t>['pareto', (3.474502202630147, -5.752794160706152, 5.752794160706151)]</t>
         </is>
       </c>
     </row>
@@ -532,27 +532,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['invgamma', (1.512925644318115, -1.4078908800515708e-28, 1.224518314017563)]</t>
+          <t>['chi2', (1.3380657374339826, -2.022860775150514e-28, 1.8494210080453803)]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['loggamma', (1.9381474601884947, -3.293518959902911e-26, 3.460459207468104)]</t>
+          <t>['gamma', (1.1060959455943804, -0.004070015051645493, 2.182753636547731)]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['beta', (1.2182841162030988, -2.040599168036255e-29, 1.6394146399666376)]</t>
+          <t>['beta', (0.8611652542892512, 79.35796489004701, -1.5419396633588808e-25, 26.695635778426045)]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['chi2', (1.3380657374339826, -2.022860775150514e-28, 1.8494210080453803)]</t>
+          <t>['beta', (1.8969335796940112, 1.1440186443623233, -1.0101306135905779, 10.760848245640155)]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['gamma', (1.8472666355219776, -3.090938143673627e-29, 1.3372897181562977)]</t>
+          <t>['invgamma', (2.030103317853264, -0.273339157562145, 1.9277887930808184)]</t>
         </is>
       </c>
     </row>
@@ -564,27 +564,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['invgauss', (1.5202481297360722, -1.1419399242669593e-27, 1.2171286359625109)]</t>
+          <t>['beta', (0.7222192851774487, 1.4655167671346607, -3.876253811786544e-29, 6.985813350784625)]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['loggamma', (1.6666258684844566, -4.0543048678170696e-26, 2.751143943389817)]</t>
+          <t>['beta', (0.8699981002941614, 1.3044457209426563, 0.08333333333330016, 5.986391159320796)]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['beta', (1.4241375370812803, -9.386663096812749e-30, 1.1419359407943657)]</t>
+          <t>['beta', (0.3021326639337568, 266.1616492102139, -2.002933488547417e-29, 70.98725221298376)]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['beta', (1.6969836415054367, -1.7474988111375316e-28, 1.5223703246488187)]</t>
+          <t>['beta', (1.9493353130904008, 1.1828119830488304, -0.7288590762220521, 7.595995794064398)]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>['beta', (5.436846358958293, -0.3628406844398816, 0.5392120278638823)]</t>
+          <t>['invgauss', (1.3223013343950307, -0.16386888664083987, 1.362835073756798)]</t>
         </is>
       </c>
     </row>

</xml_diff>